<commit_message>
Added working HMI code
</commit_message>
<xml_diff>
--- a/Modbus_Tag Table.xlsx
+++ b/Modbus_Tag Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jimke\Desktop\Embed\Alchemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87AA6760-6E49-4440-8985-58A344C1D3F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE016DE7-AD79-4AFA-8EC7-2B1F91408129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{4AD5CBED-8372-44A8-B2C4-3A6BCD43FD21}"/>
   </bookViews>
@@ -214,16 +214,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -563,7 +560,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,122 +684,122 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -813,10 +810,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -827,10 +824,10 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -841,10 +838,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -855,10 +852,10 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -869,10 +866,10 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -883,10 +880,10 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="3" t="s">

</xml_diff>